<commit_message>
Upadated and cleaned solutin helper for part II of Day Seventeen
</commit_message>
<xml_diff>
--- a/DaySeventeen/Scaffolding.xlsx
+++ b/DaySeventeen/Scaffolding.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\GitHub\AdventOfCode2019\DaySeventeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28663AE2-4CB7-4466-A7DA-459060C57BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A189E4B1-B71C-42D3-B58E-E05FC65B1623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C05E190B-C2B7-4BCD-891E-95ADD874C0B7}"/>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{12C3D709-E3BF-450C-8D28-3C26443D34A4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C05E190B-C2B7-4BCD-891E-95ADD874C0B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -64,31 +63,15 @@
   <si>
     <t>C</t>
   </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,18 +130,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,19 +150,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,11 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA520A2-5C64-484C-8DDF-87F73F9EC49F}">
   <dimension ref="A1:BA53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB40" sqref="AB40"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="1">
-      <selection activeCell="BC34" sqref="BC34:BD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,12 +2274,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87AB607-88E5-4E56-BA41-8050AD9046C0}">
-  <dimension ref="A1:AR45"/>
+  <dimension ref="A1:AP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2319,9 +2288,9 @@
     <col min="4" max="4" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="3.140625" bestFit="1" customWidth="1"/>
@@ -2343,10 +2312,9 @@
     <col min="35" max="36" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -2399,7 +2367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2427,7 +2395,7 @@
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2476,7 +2444,7 @@
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2529,7 +2497,7 @@
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2592,7 +2560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -2633,7 +2601,7 @@
       </c>
       <c r="AG6" s="3"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2650,7 +2618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
@@ -2664,7 +2632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
@@ -2680,8 +2648,11 @@
       <c r="H11" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2713,1024 +2684,120 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" t="s">
-        <v>7</v>
-      </c>
-      <c r="O15" t="s">
-        <v>10</v>
-      </c>
-      <c r="P15" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>10</v>
-      </c>
-      <c r="R15" t="s">
-        <v>9</v>
-      </c>
-      <c r="S15" t="s">
-        <v>10</v>
-      </c>
-      <c r="T15" t="s">
-        <v>8</v>
-      </c>
-      <c r="U15" t="s">
-        <v>10</v>
-      </c>
-      <c r="V15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="D16">
-        <f>CODE(D15)</f>
-        <v>65</v>
-      </c>
-      <c r="E16">
-        <f>CODE(E15)</f>
-        <v>44</v>
-      </c>
-      <c r="F16">
-        <f>CODE(F15)</f>
-        <v>66</v>
-      </c>
-      <c r="G16">
-        <f>CODE(G15)</f>
-        <v>44</v>
-      </c>
-      <c r="H16">
-        <f>CODE(H15)</f>
-        <v>65</v>
-      </c>
-      <c r="I16">
-        <f>CODE(I15)</f>
-        <v>44</v>
-      </c>
-      <c r="J16">
-        <f>CODE(J15)</f>
-        <v>67</v>
-      </c>
-      <c r="K16">
-        <f>CODE(K15)</f>
-        <v>44</v>
-      </c>
-      <c r="L16">
-        <f>CODE(L15)</f>
-        <v>67</v>
-      </c>
-      <c r="M16">
-        <f>CODE(M15)</f>
-        <v>44</v>
-      </c>
-      <c r="N16">
-        <f>CODE(N15)</f>
-        <v>65</v>
-      </c>
-      <c r="O16">
-        <f>CODE(O15)</f>
-        <v>44</v>
-      </c>
-      <c r="P16">
-        <f>CODE(P15)</f>
-        <v>66</v>
-      </c>
-      <c r="Q16">
-        <f>CODE(Q15)</f>
-        <v>44</v>
-      </c>
-      <c r="R16">
-        <f>CODE(R15)</f>
-        <v>67</v>
-      </c>
-      <c r="S16">
-        <f>CODE(S15)</f>
-        <v>44</v>
-      </c>
-      <c r="T16">
-        <f>CODE(T15)</f>
-        <v>66</v>
-      </c>
-      <c r="U16">
-        <f>CODE(U15)</f>
-        <v>44</v>
-      </c>
-      <c r="V16">
-        <f>CODE(V15)</f>
-        <v>66</v>
-      </c>
-      <c r="W16">
-        <v>10</v>
-      </c>
-      <c r="AN16" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D16:W16)</f>
-        <v>65,44,66,44,65,44,67,44,67,44,65,44,66,44,67,44,66,44,66,10</v>
-      </c>
-    </row>
-    <row r="18" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="4">
-        <v>8</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="4">
-        <v>1</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="4">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="R18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T18" s="4">
-        <v>8</v>
-      </c>
+    <row r="18" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
       <c r="U18" s="4"/>
     </row>
-    <row r="19" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D19" s="4">
-        <f>CODE(D18)</f>
-        <v>76</v>
-      </c>
-      <c r="E19" s="4">
-        <f t="shared" ref="E19:T19" si="0">CODE(E18)</f>
-        <v>44</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="N19" s="4">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="O19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="P19" s="4">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="Q19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="R19" s="4">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="S19" s="4">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="T19" s="4">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="U19" s="4">
-        <v>10</v>
-      </c>
-      <c r="AN19" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D19:W19)</f>
-        <v>76,44,56,44,82,44,49,44,48,44,76,44,56,44,82,44,56,10</v>
-      </c>
-    </row>
-    <row r="21" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="2">
-        <v>8</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P21" s="2">
-        <v>8</v>
-      </c>
+    <row r="19" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="21" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D22" s="2">
-        <f>CODE(D21)</f>
-        <v>76</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" ref="E22:P22" si="1">CODE(E21)</f>
-        <v>44</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="J22" s="2">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="M22" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="O22" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="P22" s="2">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>10</v>
-      </c>
-      <c r="AN22" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D22:W22)</f>
-        <v>76,44,49,44,50,44,82,44,56,44,82,44,56,10</v>
-      </c>
-    </row>
-    <row r="24" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="3">
-        <v>8</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="3">
-        <v>6</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N24" s="3">
-        <v>6</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R24" s="3">
-        <v>1</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
+    <row r="22" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="24" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="D25" s="3">
-        <f>CODE(D24)</f>
-        <v>76</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" ref="E25:T25" si="2">CODE(E24)</f>
-        <v>44</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="I25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="J25" s="3">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="M25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="N25" s="3">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-      <c r="O25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="P25" s="3">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="Q25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="R25" s="3">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="S25" s="3">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="T25" s="3">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="U25" s="3">
-        <v>10</v>
-      </c>
-      <c r="AN25" s="3" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D25:W25)</f>
-        <v>76,44,56,44,82,44,54,44,82,44,54,44,82,44,49,44,48,10</v>
-      </c>
+    <row r="25" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="AN25" s="3"/>
       <c r="AO25" s="3"/>
       <c r="AP25" s="3"/>
-      <c r="AQ25" s="3"/>
-      <c r="AR25" s="3"/>
-    </row>
-    <row r="27" spans="4:44" x14ac:dyDescent="0.25">
-      <c r="AN27" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(",",,AN16,AN19,AN22,AN25)</f>
-        <v>65,44,66,44,65,44,67,44,67,44,65,44,66,44,67,44,66,44,66,10,76,44,56,44,82,44,49,44,48,44,76,44,56,44,82,44,56,10,76,44,49,44,50,44,82,44,56,44,82,44,56,10,76,44,56,44,82,44,54,44,82,44,54,44,82,44,49,44,48,10</v>
-      </c>
-    </row>
-    <row r="33" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K33" t="s">
-        <v>10</v>
-      </c>
-      <c r="L33" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" t="s">
-        <v>10</v>
-      </c>
-      <c r="N33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O33" t="s">
-        <v>10</v>
-      </c>
-      <c r="P33" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>10</v>
-      </c>
-      <c r="R33" t="s">
-        <v>9</v>
-      </c>
-      <c r="S33" t="s">
-        <v>10</v>
-      </c>
-      <c r="T33" t="s">
-        <v>8</v>
-      </c>
-      <c r="U33" t="s">
-        <v>10</v>
-      </c>
-      <c r="V33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <f>CODE(D33)</f>
-        <v>65</v>
-      </c>
-      <c r="E34">
-        <f>CODE(E33)</f>
-        <v>44</v>
-      </c>
-      <c r="F34">
-        <f>CODE(F33)</f>
-        <v>66</v>
-      </c>
-      <c r="G34">
-        <f>CODE(G33)</f>
-        <v>44</v>
-      </c>
-      <c r="H34">
-        <f>CODE(H33)</f>
-        <v>65</v>
-      </c>
-      <c r="I34">
-        <f>CODE(I33)</f>
-        <v>44</v>
-      </c>
-      <c r="J34">
-        <f>CODE(J33)</f>
-        <v>67</v>
-      </c>
-      <c r="K34">
-        <f>CODE(K33)</f>
-        <v>44</v>
-      </c>
-      <c r="L34">
-        <f>CODE(L33)</f>
-        <v>67</v>
-      </c>
-      <c r="M34">
-        <f>CODE(M33)</f>
-        <v>44</v>
-      </c>
-      <c r="N34">
-        <f>CODE(N33)</f>
-        <v>65</v>
-      </c>
-      <c r="O34">
-        <f>CODE(O33)</f>
-        <v>44</v>
-      </c>
-      <c r="P34">
-        <f>CODE(P33)</f>
-        <v>66</v>
-      </c>
-      <c r="Q34">
-        <f>CODE(Q33)</f>
-        <v>44</v>
-      </c>
-      <c r="R34">
-        <f>CODE(R33)</f>
-        <v>67</v>
-      </c>
-      <c r="S34">
-        <f>CODE(S33)</f>
-        <v>44</v>
-      </c>
-      <c r="T34">
-        <f>CODE(T33)</f>
-        <v>66</v>
-      </c>
-      <c r="U34">
-        <f>CODE(U33)</f>
-        <v>44</v>
-      </c>
-      <c r="V34">
-        <f>CODE(V33)</f>
-        <v>66</v>
-      </c>
-      <c r="W34">
-        <v>10</v>
-      </c>
-      <c r="AN34" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D34:W34)</f>
-        <v>65,44,66,44,65,44,67,44,67,44,65,44,66,44,67,44,66,44,66,10</v>
-      </c>
-    </row>
-    <row r="36" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="4">
-        <v>8</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="4">
-        <v>1</v>
-      </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="4">
-        <v>0</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="O36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P36" s="4">
-        <v>8</v>
-      </c>
-      <c r="Q36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="R36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T36" s="4">
-        <v>8</v>
-      </c>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D37" s="4">
-        <f>CODE(D36)</f>
-        <v>76</v>
-      </c>
-      <c r="E37" s="4">
-        <f t="shared" ref="E37" si="3">CODE(E36)</f>
-        <v>44</v>
-      </c>
-      <c r="F37" s="4">
-        <f t="shared" ref="F37" si="4">CODE(F36)</f>
-        <v>56</v>
-      </c>
-      <c r="G37" s="4">
-        <f t="shared" ref="G37" si="5">CODE(G36)</f>
-        <v>44</v>
-      </c>
-      <c r="H37" s="4">
-        <f t="shared" ref="H37" si="6">CODE(H36)</f>
-        <v>82</v>
-      </c>
-      <c r="I37" s="4">
-        <f t="shared" ref="I37" si="7">CODE(I36)</f>
-        <v>44</v>
-      </c>
-      <c r="J37" s="4">
-        <f t="shared" ref="J37" si="8">CODE(J36)</f>
-        <v>49</v>
-      </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="4">
-        <f t="shared" ref="L37" si="9">CODE(L36)</f>
-        <v>48</v>
-      </c>
-      <c r="M37" s="4">
-        <f t="shared" ref="M37" si="10">CODE(M36)</f>
-        <v>44</v>
-      </c>
-      <c r="N37" s="4">
-        <f t="shared" ref="N37" si="11">CODE(N36)</f>
-        <v>76</v>
-      </c>
-      <c r="O37" s="4">
-        <f t="shared" ref="O37" si="12">CODE(O36)</f>
-        <v>44</v>
-      </c>
-      <c r="P37" s="4">
-        <f t="shared" ref="P37" si="13">CODE(P36)</f>
-        <v>56</v>
-      </c>
-      <c r="Q37" s="4">
-        <f t="shared" ref="Q37" si="14">CODE(Q36)</f>
-        <v>44</v>
-      </c>
-      <c r="R37" s="4">
-        <f t="shared" ref="R37" si="15">CODE(R36)</f>
-        <v>82</v>
-      </c>
-      <c r="S37" s="4">
-        <f t="shared" ref="S37" si="16">CODE(S36)</f>
-        <v>44</v>
-      </c>
-      <c r="T37" s="4">
-        <f t="shared" ref="T37" si="17">CODE(T36)</f>
-        <v>56</v>
-      </c>
-      <c r="U37" s="4">
-        <v>10</v>
-      </c>
-      <c r="AN37" s="4" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D37:W37)</f>
-        <v>76,44,56,44,82,44,49,48,44,76,44,56,44,82,44,56,10</v>
-      </c>
-    </row>
-    <row r="39" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="2">
-        <v>1</v>
-      </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="2">
-        <v>2</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L39" s="2">
-        <v>8</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P39" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q39" s="2"/>
-    </row>
-    <row r="40" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D40" s="2">
-        <f>CODE(D39)</f>
-        <v>76</v>
-      </c>
-      <c r="E40" s="2">
-        <f t="shared" ref="E40" si="18">CODE(E39)</f>
-        <v>44</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" ref="F40" si="19">CODE(F39)</f>
-        <v>49</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="2">
-        <f t="shared" ref="H40" si="20">CODE(H39)</f>
-        <v>50</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" ref="I40" si="21">CODE(I39)</f>
-        <v>44</v>
-      </c>
-      <c r="J40" s="2">
-        <f t="shared" ref="J40" si="22">CODE(J39)</f>
-        <v>82</v>
-      </c>
-      <c r="K40" s="2">
-        <f t="shared" ref="K40" si="23">CODE(K39)</f>
-        <v>44</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" ref="L40" si="24">CODE(L39)</f>
-        <v>56</v>
-      </c>
-      <c r="M40" s="2">
-        <f t="shared" ref="M40" si="25">CODE(M39)</f>
-        <v>44</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" ref="N40" si="26">CODE(N39)</f>
-        <v>82</v>
-      </c>
-      <c r="O40" s="2">
-        <f t="shared" ref="O40" si="27">CODE(O39)</f>
-        <v>44</v>
-      </c>
-      <c r="P40" s="2">
-        <f t="shared" ref="P40" si="28">CODE(P39)</f>
-        <v>56</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>10</v>
-      </c>
-      <c r="AN40" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D40:W40)</f>
-        <v>76,44,49,50,44,82,44,56,44,82,44,56,10</v>
-      </c>
-    </row>
-    <row r="42" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="3">
-        <v>8</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J42" s="3">
-        <v>6</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N42" s="3">
-        <v>6</v>
-      </c>
-      <c r="O42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R42" s="3">
-        <v>1</v>
-      </c>
-      <c r="S42" s="10"/>
-      <c r="T42" s="3">
-        <v>0</v>
-      </c>
-      <c r="U42" s="3"/>
-    </row>
-    <row r="43" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="D43" s="3">
-        <f>CODE(D42)</f>
-        <v>76</v>
-      </c>
-      <c r="E43" s="3">
-        <f t="shared" ref="E43" si="29">CODE(E42)</f>
-        <v>44</v>
-      </c>
-      <c r="F43" s="3">
-        <f t="shared" ref="F43" si="30">CODE(F42)</f>
-        <v>56</v>
-      </c>
-      <c r="G43" s="3">
-        <f t="shared" ref="G43" si="31">CODE(G42)</f>
-        <v>44</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" ref="H43" si="32">CODE(H42)</f>
-        <v>82</v>
-      </c>
-      <c r="I43" s="3">
-        <f t="shared" ref="I43" si="33">CODE(I42)</f>
-        <v>44</v>
-      </c>
-      <c r="J43" s="3">
-        <f t="shared" ref="J43" si="34">CODE(J42)</f>
-        <v>54</v>
-      </c>
-      <c r="K43" s="3">
-        <f t="shared" ref="K43" si="35">CODE(K42)</f>
-        <v>44</v>
-      </c>
-      <c r="L43" s="3">
-        <f t="shared" ref="L43" si="36">CODE(L42)</f>
-        <v>82</v>
-      </c>
-      <c r="M43" s="3">
-        <f t="shared" ref="M43" si="37">CODE(M42)</f>
-        <v>44</v>
-      </c>
-      <c r="N43" s="3">
-        <f t="shared" ref="N43" si="38">CODE(N42)</f>
-        <v>54</v>
-      </c>
-      <c r="O43" s="3">
-        <f t="shared" ref="O43" si="39">CODE(O42)</f>
-        <v>44</v>
-      </c>
-      <c r="P43" s="3">
-        <f t="shared" ref="P43" si="40">CODE(P42)</f>
-        <v>82</v>
-      </c>
-      <c r="Q43" s="3">
-        <f t="shared" ref="Q43" si="41">CODE(Q42)</f>
-        <v>44</v>
-      </c>
-      <c r="R43" s="3">
-        <f t="shared" ref="R43" si="42">CODE(R42)</f>
-        <v>49</v>
-      </c>
-      <c r="S43" s="10"/>
-      <c r="T43" s="3">
-        <f t="shared" ref="T43" si="43">CODE(T42)</f>
-        <v>48</v>
-      </c>
-      <c r="U43" s="3">
-        <v>10</v>
-      </c>
-      <c r="AN43" s="3" t="str">
-        <f>_xlfn.TEXTJOIN(",",,D43:W43)</f>
-        <v>76,44,56,44,82,44,54,44,82,44,54,44,82,44,49,48,10</v>
-      </c>
-    </row>
-    <row r="45" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AN45" s="11" t="str">
-        <f>_xlfn.TEXTJOIN(",",,AN34,AN37,AN40,AN43)</f>
-        <v>65,44,66,44,65,44,67,44,67,44,65,44,66,44,67,44,66,44,66,10,76,44,56,44,82,44,49,48,44,76,44,56,44,82,44,56,10,76,44,49,50,44,82,44,56,44,82,44,56,10,76,44,56,44,82,44,54,44,82,44,54,44,82,44,49,48,10</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>